<commit_message>
v2.3 league dashboard acabado: mejoras visuales, ranking, animación, selección de equipo, cuadrantes, logos, y experiencia de usuario finalizada
</commit_message>
<xml_diff>
--- a/Datos/Wyscout Liga/Team Stats Barcelona.xlsx
+++ b/Datos/Wyscout Liga/Team Stats Barcelona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyadb\Documents\tfm\Datos\Wyscout Liga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3661A59C-F645-4A3F-9466-AEF2697D8A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B0C90D-79F7-4389-BC5A-10462250AAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -874,8 +874,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DF119"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A102" zoomScale="86" workbookViewId="0">
-      <selection activeCell="BF91" activeCellId="2" sqref="A70:XFD70 A74:XFD74 A91:XFD91"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="B1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1344,130 +1344,130 @@
       <c r="I1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AX1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AY1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="AZ1" s="2" t="s">
@@ -1476,25 +1476,25 @@
       <c r="BA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BB1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BC1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BD1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="BE1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BF1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BG1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BH1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="BI1" s="2" t="s">
@@ -1503,40 +1503,40 @@
       <c r="BJ1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BK1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BL1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BM1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BN1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BO1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BP1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BR1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BS1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BT1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BU1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BV1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="BW1" s="2" t="s">
@@ -1554,76 +1554,76 @@
       <c r="CA1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CB1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CC1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CD1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CE1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CF1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CG1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CH1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CI1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CK1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="CL1" s="4" t="s">
+      <c r="CL1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CM1" s="4" t="s">
+      <c r="CM1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CN1" s="4" t="s">
+      <c r="CN1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="CO1" s="4" t="s">
+      <c r="CO1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CP1" s="4" t="s">
+      <c r="CP1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CQ1" s="4" t="s">
+      <c r="CQ1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="CR1" s="4" t="s">
+      <c r="CR1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CS1" s="4" t="s">
+      <c r="CS1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CT1" s="4" t="s">
+      <c r="CT1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="CU1" s="4" t="s">
+      <c r="CU1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CV1" s="4" t="s">
+      <c r="CV1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CW1" s="4" t="s">
+      <c r="CW1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="CX1" s="4" t="s">
+      <c r="CX1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="CY1" s="4" t="s">
+      <c r="CY1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="CZ1" s="2" t="s">
@@ -2501,16 +2501,16 @@
       </c>
     </row>
     <row r="4" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>101</v>
       </c>
       <c r="E4" t="s">
@@ -2526,7 +2526,7 @@
         <v>1.53</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I24" si="7">BJ4+(BL4-BJ4)*0.3</f>
+        <f t="shared" ref="I4" si="7">BJ4+(BL4-BJ4)*0.3</f>
         <v>2</v>
       </c>
       <c r="J4">
@@ -2834,16 +2834,16 @@
       </c>
     </row>
     <row r="5" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>101</v>
       </c>
       <c r="E5" t="s">
@@ -2859,7 +2859,7 @@
         <v>0.79</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I24" si="8">BJ5+(BK5-BJ5)*0.3</f>
+        <f t="shared" ref="I5" si="8">BJ5+(BK5-BJ5)*0.3</f>
         <v>7</v>
       </c>
       <c r="J5">
@@ -3167,16 +3167,16 @@
       </c>
     </row>
     <row r="6" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>95</v>
       </c>
       <c r="E6" t="s">
@@ -3192,7 +3192,7 @@
         <v>2.82</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I6:I24" si="9">BJ6+(BL6-BJ6)*0.3</f>
+        <f t="shared" ref="I6" si="9">BJ6+(BL6-BJ6)*0.3</f>
         <v>1.3</v>
       </c>
       <c r="J6">
@@ -3500,16 +3500,16 @@
       </c>
     </row>
     <row r="7" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>95</v>
       </c>
       <c r="E7" t="s">
@@ -3525,7 +3525,7 @@
         <v>1.02</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" ref="I7:I24" si="10">BJ7+(BK7-BJ7)*0.3</f>
+        <f t="shared" ref="I7" si="10">BJ7+(BK7-BJ7)*0.3</f>
         <v>7.5</v>
       </c>
       <c r="J7">
@@ -3833,16 +3833,16 @@
       </c>
     </row>
     <row r="8" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>103</v>
       </c>
       <c r="E8" t="s">
@@ -3858,7 +3858,7 @@
         <v>1.85</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ref="I8:I24" si="11">BJ8+(BL8-BJ8)*0.3</f>
+        <f t="shared" ref="I8" si="11">BJ8+(BL8-BJ8)*0.3</f>
         <v>2.4</v>
       </c>
       <c r="J8">
@@ -4166,16 +4166,16 @@
       </c>
     </row>
     <row r="9" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>103</v>
       </c>
       <c r="E9" t="s">
@@ -4191,7 +4191,7 @@
         <v>3.07</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" ref="I9:I24" si="12">BJ9+(BK9-BJ9)*0.3</f>
+        <f t="shared" ref="I9" si="12">BJ9+(BK9-BJ9)*0.3</f>
         <v>3.6999999999999997</v>
       </c>
       <c r="J9">
@@ -4499,16 +4499,16 @@
       </c>
     </row>
     <row r="10" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <v>94</v>
       </c>
       <c r="E10" t="s">
@@ -4524,7 +4524,7 @@
         <v>3.64</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" ref="I10:I24" si="13">BJ10+(BL10-BJ10)*0.3</f>
+        <f t="shared" ref="I10" si="13">BJ10+(BL10-BJ10)*0.3</f>
         <v>0</v>
       </c>
       <c r="J10">
@@ -4832,16 +4832,16 @@
       </c>
     </row>
     <row r="11" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="4">
         <v>94</v>
       </c>
       <c r="E11" t="s">
@@ -4857,7 +4857,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" ref="I11:I24" si="14">BJ11+(BK11-BJ11)*0.3</f>
+        <f t="shared" ref="I11" si="14">BJ11+(BK11-BJ11)*0.3</f>
         <v>12.4</v>
       </c>
       <c r="J11">
@@ -5165,16 +5165,16 @@
       </c>
     </row>
     <row r="12" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="4">
         <v>101</v>
       </c>
       <c r="E12" t="s">
@@ -5190,7 +5190,7 @@
         <v>2.68</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" ref="I12:I24" si="15">BJ12+(BL12-BJ12)*0.3</f>
+        <f t="shared" ref="I12" si="15">BJ12+(BL12-BJ12)*0.3</f>
         <v>4.9000000000000004</v>
       </c>
       <c r="J12">
@@ -5498,16 +5498,16 @@
       </c>
     </row>
     <row r="13" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="4">
         <v>101</v>
       </c>
       <c r="E13" t="s">
@@ -5523,7 +5523,7 @@
         <v>1.44</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" ref="I13:I24" si="16">BJ13+(BK13-BJ13)*0.3</f>
+        <f t="shared" ref="I13" si="16">BJ13+(BK13-BJ13)*0.3</f>
         <v>7.9</v>
       </c>
       <c r="J13">
@@ -5831,16 +5831,16 @@
       </c>
     </row>
     <row r="14" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="4">
         <v>99</v>
       </c>
       <c r="E14" t="s">
@@ -5856,7 +5856,7 @@
         <v>1.85</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" ref="I14:I24" si="17">BJ14+(BL14-BJ14)*0.3</f>
+        <f t="shared" ref="I14" si="17">BJ14+(BL14-BJ14)*0.3</f>
         <v>0.6</v>
       </c>
       <c r="J14">
@@ -6164,16 +6164,16 @@
       </c>
     </row>
     <row r="15" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="4">
         <v>99</v>
       </c>
       <c r="E15" t="s">
@@ -6189,7 +6189,7 @@
         <v>0.79</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" ref="I15:I24" si="18">BJ15+(BK15-BJ15)*0.3</f>
+        <f t="shared" ref="I15" si="18">BJ15+(BK15-BJ15)*0.3</f>
         <v>6.2</v>
       </c>
       <c r="J15">
@@ -6497,16 +6497,16 @@
       </c>
     </row>
     <row r="16" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="4">
         <v>99</v>
       </c>
       <c r="E16" t="s">
@@ -6522,7 +6522,7 @@
         <v>2.62</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" ref="I16:I24" si="19">BJ16+(BL16-BJ16)*0.3</f>
+        <f t="shared" ref="I16" si="19">BJ16+(BL16-BJ16)*0.3</f>
         <v>1.2</v>
       </c>
       <c r="J16">
@@ -6830,16 +6830,16 @@
       </c>
     </row>
     <row r="17" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="4">
         <v>99</v>
       </c>
       <c r="E17" t="s">
@@ -6855,7 +6855,7 @@
         <v>0.94</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" ref="I17:I24" si="20">BJ17+(BK17-BJ17)*0.3</f>
+        <f t="shared" ref="I17" si="20">BJ17+(BK17-BJ17)*0.3</f>
         <v>4.9000000000000004</v>
       </c>
       <c r="J17">
@@ -7163,16 +7163,16 @@
       </c>
     </row>
     <row r="18" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="4">
         <v>100</v>
       </c>
       <c r="E18" t="s">
@@ -7188,7 +7188,7 @@
         <v>1.89</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" ref="I18:I24" si="21">BJ18+(BL18-BJ18)*0.3</f>
+        <f t="shared" ref="I18" si="21">BJ18+(BL18-BJ18)*0.3</f>
         <v>1.9</v>
       </c>
       <c r="J18">
@@ -7496,16 +7496,16 @@
       </c>
     </row>
     <row r="19" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="4">
         <v>100</v>
       </c>
       <c r="E19" t="s">
@@ -7521,7 +7521,7 @@
         <v>0.94</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" ref="I19:I24" si="22">BJ19+(BK19-BJ19)*0.3</f>
+        <f t="shared" ref="I19" si="22">BJ19+(BK19-BJ19)*0.3</f>
         <v>5.8</v>
       </c>
       <c r="J19">
@@ -7829,16 +7829,16 @@
       </c>
     </row>
     <row r="20" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="4">
         <v>92</v>
       </c>
       <c r="E20" t="s">
@@ -7854,7 +7854,7 @@
         <v>2.9</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" ref="I20:I24" si="23">BJ20+(BL20-BJ20)*0.3</f>
+        <f t="shared" ref="I20" si="23">BJ20+(BL20-BJ20)*0.3</f>
         <v>0.3</v>
       </c>
       <c r="J20">
@@ -8162,16 +8162,16 @@
       </c>
     </row>
     <row r="21" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="4">
         <v>92</v>
       </c>
       <c r="E21" t="s">
@@ -8187,7 +8187,7 @@
         <v>0.08</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" ref="I21:I24" si="24">BJ21+(BK21-BJ21)*0.3</f>
+        <f t="shared" ref="I21" si="24">BJ21+(BK21-BJ21)*0.3</f>
         <v>8.6</v>
       </c>
       <c r="J21">
@@ -8495,16 +8495,16 @@
       </c>
     </row>
     <row r="22" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="4">
         <v>100</v>
       </c>
       <c r="E22" t="s">
@@ -8520,7 +8520,7 @@
         <v>1.25</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" ref="I22:I24" si="25">BJ22+(BL22-BJ22)*0.3</f>
+        <f t="shared" ref="I22" si="25">BJ22+(BL22-BJ22)*0.3</f>
         <v>0</v>
       </c>
       <c r="J22">
@@ -8828,16 +8828,16 @@
       </c>
     </row>
     <row r="23" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="4">
         <v>100</v>
       </c>
       <c r="E23" t="s">
@@ -8853,7 +8853,7 @@
         <v>0.09</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" ref="I23:I24" si="26">BJ23+(BK23-BJ23)*0.3</f>
+        <f t="shared" ref="I23" si="26">BJ23+(BK23-BJ23)*0.3</f>
         <v>4</v>
       </c>
       <c r="J23">
@@ -9161,16 +9161,16 @@
       </c>
     </row>
     <row r="24" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="4">
         <v>99</v>
       </c>
       <c r="E24" t="s">
@@ -9494,16 +9494,16 @@
       </c>
     </row>
     <row r="25" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="4">
         <v>99</v>
       </c>
       <c r="E25" t="s">
@@ -9827,16 +9827,16 @@
       </c>
     </row>
     <row r="26" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="4">
         <v>96</v>
       </c>
       <c r="E26" t="s">
@@ -9852,7 +9852,7 @@
         <v>3.47</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" ref="I26:I57" si="28">BJ26+(BK26-BJ26)*0.3</f>
+        <f t="shared" ref="I26" si="28">BJ26+(BK26-BJ26)*0.3</f>
         <v>2.5</v>
       </c>
       <c r="J26">
@@ -10160,16 +10160,16 @@
       </c>
     </row>
     <row r="27" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="4">
         <v>96</v>
       </c>
       <c r="E27" t="s">
@@ -10185,7 +10185,7 @@
         <v>1.05</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" ref="I27:I90" si="29">BJ27+(BL27-BJ27)*0.3</f>
+        <f t="shared" ref="I27:I73" si="29">BJ27+(BL27-BJ27)*0.3</f>
         <v>8.5</v>
       </c>
       <c r="J27">
@@ -10493,16 +10493,16 @@
       </c>
     </row>
     <row r="28" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="4">
         <v>102</v>
       </c>
       <c r="E28" t="s">
@@ -10518,7 +10518,7 @@
         <v>3.39</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" ref="I28:I91" si="30">BJ28+(BK28-BJ28)*0.3</f>
+        <f t="shared" ref="I28:I74" si="30">BJ28+(BK28-BJ28)*0.3</f>
         <v>5.8</v>
       </c>
       <c r="J28">
@@ -10826,16 +10826,16 @@
       </c>
     </row>
     <row r="29" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="4">
         <v>102</v>
       </c>
       <c r="E29" t="s">
@@ -10851,7 +10851,7 @@
         <v>2.78</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" ref="I29:I92" si="31">BJ29+(BL29-BJ29)*0.3</f>
+        <f t="shared" ref="I29:I75" si="31">BJ29+(BL29-BJ29)*0.3</f>
         <v>6.8</v>
       </c>
       <c r="J29">
@@ -11159,16 +11159,16 @@
       </c>
     </row>
     <row r="30" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="4">
         <v>100</v>
       </c>
       <c r="E30" t="s">
@@ -11184,7 +11184,7 @@
         <v>1.73</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" ref="I30:I93" si="32">BJ30+(BK30-BJ30)*0.3</f>
+        <f t="shared" ref="I30:I76" si="32">BJ30+(BK30-BJ30)*0.3</f>
         <v>3.1</v>
       </c>
       <c r="J30">
@@ -11492,16 +11492,16 @@
       </c>
     </row>
     <row r="31" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="4">
         <v>100</v>
       </c>
       <c r="E31" t="s">
@@ -11517,7 +11517,7 @@
         <v>1.6</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" ref="I31:I94" si="33">BJ31+(BL31-BJ31)*0.3</f>
+        <f t="shared" ref="I31:I77" si="33">BJ31+(BL31-BJ31)*0.3</f>
         <v>1.9</v>
       </c>
       <c r="J31">
@@ -11825,16 +11825,16 @@
       </c>
     </row>
     <row r="32" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="4">
         <v>95</v>
       </c>
       <c r="E32" t="s">
@@ -11850,7 +11850,7 @@
         <v>2.88</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" ref="I32:I95" si="34">BJ32+(BK32-BJ32)*0.3</f>
+        <f t="shared" ref="I32:I78" si="34">BJ32+(BK32-BJ32)*0.3</f>
         <v>2.8</v>
       </c>
       <c r="J32">
@@ -12158,16 +12158,16 @@
       </c>
     </row>
     <row r="33" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="4">
         <v>95</v>
       </c>
       <c r="E33" t="s">
@@ -12183,7 +12183,7 @@
         <v>1.66</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" ref="I33:I96" si="35">BJ33+(BL33-BJ33)*0.3</f>
+        <f t="shared" ref="I33:I79" si="35">BJ33+(BL33-BJ33)*0.3</f>
         <v>6.2</v>
       </c>
       <c r="J33">
@@ -12491,16 +12491,16 @@
       </c>
     </row>
     <row r="34" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="4">
         <v>108</v>
       </c>
       <c r="E34" t="s">
@@ -12516,7 +12516,7 @@
         <v>2.2200000000000002</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" ref="I34:I97" si="36">BJ34+(BK34-BJ34)*0.3</f>
+        <f t="shared" ref="I34:I80" si="36">BJ34+(BK34-BJ34)*0.3</f>
         <v>6.5</v>
       </c>
       <c r="J34">
@@ -12824,16 +12824,16 @@
       </c>
     </row>
     <row r="35" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="4">
         <v>108</v>
       </c>
       <c r="E35" t="s">
@@ -12849,7 +12849,7 @@
         <v>1.49</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" ref="I35:I98" si="37">BJ35+(BL35-BJ35)*0.3</f>
+        <f t="shared" ref="I35:I81" si="37">BJ35+(BL35-BJ35)*0.3</f>
         <v>5.9</v>
       </c>
       <c r="J35">
@@ -13157,16 +13157,16 @@
       </c>
     </row>
     <row r="36" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="4">
         <v>99</v>
       </c>
       <c r="E36" t="s">
@@ -13182,7 +13182,7 @@
         <v>2.57</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" ref="I36:I99" si="38">BJ36+(BK36-BJ36)*0.3</f>
+        <f t="shared" ref="I36:I82" si="38">BJ36+(BK36-BJ36)*0.3</f>
         <v>2.6999999999999997</v>
       </c>
       <c r="J36">
@@ -13490,16 +13490,16 @@
       </c>
     </row>
     <row r="37" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="4">
         <v>99</v>
       </c>
       <c r="E37" t="s">
@@ -13515,7 +13515,7 @@
         <v>0.74</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" ref="I37:I100" si="39">BJ37+(BL37-BJ37)*0.3</f>
+        <f t="shared" ref="I37:I83" si="39">BJ37+(BL37-BJ37)*0.3</f>
         <v>3.8</v>
       </c>
       <c r="J37">
@@ -13823,16 +13823,16 @@
       </c>
     </row>
     <row r="38" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="4">
         <v>93</v>
       </c>
       <c r="E38" t="s">
@@ -13848,7 +13848,7 @@
         <v>3.59</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" ref="I38:I101" si="40">BJ38+(BK38-BJ38)*0.3</f>
+        <f t="shared" ref="I38:I84" si="40">BJ38+(BK38-BJ38)*0.3</f>
         <v>0.6</v>
       </c>
       <c r="J38">
@@ -14156,16 +14156,16 @@
       </c>
     </row>
     <row r="39" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="4">
         <v>93</v>
       </c>
       <c r="E39" t="s">
@@ -14181,7 +14181,7 @@
         <v>0.04</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" ref="I39:I102" si="41">BJ39+(BL39-BJ39)*0.3</f>
+        <f t="shared" ref="I39:I85" si="41">BJ39+(BL39-BJ39)*0.3</f>
         <v>5.8</v>
       </c>
       <c r="J39">
@@ -14489,16 +14489,16 @@
       </c>
     </row>
     <row r="40" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="4">
         <v>99</v>
       </c>
       <c r="E40" t="s">
@@ -14514,7 +14514,7 @@
         <v>2.29</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" ref="I40:I103" si="42">BJ40+(BK40-BJ40)*0.3</f>
+        <f t="shared" ref="I40:I86" si="42">BJ40+(BK40-BJ40)*0.3</f>
         <v>2.9</v>
       </c>
       <c r="J40">
@@ -14822,16 +14822,16 @@
       </c>
     </row>
     <row r="41" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="4">
         <v>99</v>
       </c>
       <c r="E41" t="s">
@@ -14847,7 +14847,7 @@
         <v>0.52</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" ref="I41:I104" si="43">BJ41+(BL41-BJ41)*0.3</f>
+        <f t="shared" ref="I41:I87" si="43">BJ41+(BL41-BJ41)*0.3</f>
         <v>2.5</v>
       </c>
       <c r="J41">
@@ -15155,16 +15155,16 @@
       </c>
     </row>
     <row r="42" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="4">
         <v>101</v>
       </c>
       <c r="E42" t="s">
@@ -15180,7 +15180,7 @@
         <v>2.72</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" ref="I42:I105" si="44">BJ42+(BK42-BJ42)*0.3</f>
+        <f t="shared" ref="I42:I88" si="44">BJ42+(BK42-BJ42)*0.3</f>
         <v>2.5</v>
       </c>
       <c r="J42">
@@ -15488,16 +15488,16 @@
       </c>
     </row>
     <row r="43" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="4">
         <v>101</v>
       </c>
       <c r="E43" t="s">
@@ -15513,7 +15513,7 @@
         <v>0.43</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" ref="I43:I106" si="45">BJ43+(BL43-BJ43)*0.3</f>
+        <f t="shared" ref="I43:I89" si="45">BJ43+(BL43-BJ43)*0.3</f>
         <v>0.89999999999999991</v>
       </c>
       <c r="J43">
@@ -15821,16 +15821,16 @@
       </c>
     </row>
     <row r="44" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="4">
         <v>97</v>
       </c>
       <c r="E44" t="s">
@@ -15846,7 +15846,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" ref="I44:I107" si="46">BJ44+(BK44-BJ44)*0.3</f>
+        <f t="shared" ref="I44:I90" si="46">BJ44+(BK44-BJ44)*0.3</f>
         <v>5.3</v>
       </c>
       <c r="J44">
@@ -16154,16 +16154,16 @@
       </c>
     </row>
     <row r="45" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="4">
         <v>97</v>
       </c>
       <c r="E45" t="s">
@@ -16179,7 +16179,7 @@
         <v>2.52</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" ref="I45:I108" si="47">BJ45+(BL45-BJ45)*0.3</f>
+        <f t="shared" ref="I45:I91" si="47">BJ45+(BL45-BJ45)*0.3</f>
         <v>4.5</v>
       </c>
       <c r="J45">
@@ -16487,16 +16487,16 @@
       </c>
     </row>
     <row r="46" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="4">
         <v>103</v>
       </c>
       <c r="E46" t="s">
@@ -16512,7 +16512,7 @@
         <v>1.06</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" ref="I46:I109" si="48">BJ46+(BK46-BJ46)*0.3</f>
+        <f t="shared" ref="I46:I92" si="48">BJ46+(BK46-BJ46)*0.3</f>
         <v>4.6999999999999993</v>
       </c>
       <c r="J46">
@@ -16820,16 +16820,16 @@
       </c>
     </row>
     <row r="47" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="4">
         <v>103</v>
       </c>
       <c r="E47" t="s">
@@ -16845,7 +16845,7 @@
         <v>3.02</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" ref="I47:I110" si="49">BJ47+(BL47-BJ47)*0.3</f>
+        <f t="shared" ref="I47:I94" si="49">BJ47+(BL47-BJ47)*0.3</f>
         <v>2.6</v>
       </c>
       <c r="J47">
@@ -17153,16 +17153,16 @@
       </c>
     </row>
     <row r="48" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="4">
         <v>95</v>
       </c>
       <c r="E48" t="s">
@@ -17486,16 +17486,16 @@
       </c>
     </row>
     <row r="49" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="4">
         <v>95</v>
       </c>
       <c r="E49" t="s">
@@ -17511,7 +17511,7 @@
         <v>0.6</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" ref="I49:I80" si="50">BJ49+(BK49-BJ49)*0.3</f>
+        <f t="shared" ref="I49" si="50">BJ49+(BK49-BJ49)*0.3</f>
         <v>9.5</v>
       </c>
       <c r="J49">
@@ -17819,16 +17819,16 @@
       </c>
     </row>
     <row r="50" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="4">
         <v>102</v>
       </c>
       <c r="E50" t="s">
@@ -18152,16 +18152,16 @@
       </c>
     </row>
     <row r="51" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="4">
         <v>102</v>
       </c>
       <c r="E51" t="s">
@@ -18485,16 +18485,16 @@
       </c>
     </row>
     <row r="52" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="4">
         <v>94</v>
       </c>
       <c r="E52" t="s">
@@ -18818,16 +18818,16 @@
       </c>
     </row>
     <row r="53" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="4">
         <v>94</v>
       </c>
       <c r="E53" t="s">
@@ -19151,16 +19151,16 @@
       </c>
     </row>
     <row r="54" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="4">
         <v>97</v>
       </c>
       <c r="E54" t="s">
@@ -19484,16 +19484,16 @@
       </c>
     </row>
     <row r="55" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="4">
         <v>97</v>
       </c>
       <c r="E55" t="s">
@@ -19817,16 +19817,16 @@
       </c>
     </row>
     <row r="56" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="4">
         <v>98</v>
       </c>
       <c r="E56" t="s">
@@ -20150,16 +20150,16 @@
       </c>
     </row>
     <row r="57" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="4">
         <v>98</v>
       </c>
       <c r="E57" t="s">
@@ -20483,16 +20483,16 @@
       </c>
     </row>
     <row r="58" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="4">
         <v>98</v>
       </c>
       <c r="E58" t="s">
@@ -20816,16 +20816,16 @@
       </c>
     </row>
     <row r="59" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="4">
         <v>98</v>
       </c>
       <c r="E59" t="s">
@@ -21149,16 +21149,16 @@
       </c>
     </row>
     <row r="60" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="4">
         <v>100</v>
       </c>
       <c r="E60" t="s">
@@ -21482,16 +21482,16 @@
       </c>
     </row>
     <row r="61" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="4">
         <v>100</v>
       </c>
       <c r="E61" t="s">
@@ -21815,16 +21815,16 @@
       </c>
     </row>
     <row r="62" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="4">
         <v>94</v>
       </c>
       <c r="E62" t="s">
@@ -22148,16 +22148,16 @@
       </c>
     </row>
     <row r="63" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="4">
         <v>94</v>
       </c>
       <c r="E63" t="s">
@@ -22481,16 +22481,16 @@
       </c>
     </row>
     <row r="64" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="4">
         <v>95</v>
       </c>
       <c r="E64" t="s">
@@ -22814,16 +22814,16 @@
       </c>
     </row>
     <row r="65" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="4">
         <v>95</v>
       </c>
       <c r="E65" t="s">
@@ -23147,16 +23147,16 @@
       </c>
     </row>
     <row r="66" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="4">
         <v>97</v>
       </c>
       <c r="E66" t="s">
@@ -23480,16 +23480,16 @@
       </c>
     </row>
     <row r="67" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="4">
         <v>97</v>
       </c>
       <c r="E67" t="s">
@@ -23813,16 +23813,16 @@
       </c>
     </row>
     <row r="68" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="4">
         <v>98</v>
       </c>
       <c r="E68" t="s">
@@ -24146,16 +24146,16 @@
       </c>
     </row>
     <row r="69" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="4">
         <v>98</v>
       </c>
       <c r="E69" t="s">
@@ -24479,16 +24479,16 @@
       </c>
     </row>
     <row r="70" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D70" s="3">
+      <c r="D70" s="4">
         <v>95</v>
       </c>
       <c r="E70" t="s">
@@ -24812,16 +24812,16 @@
       </c>
     </row>
     <row r="71" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D71" s="4">
         <v>95</v>
       </c>
       <c r="E71" t="s">
@@ -25145,16 +25145,16 @@
       </c>
     </row>
     <row r="72" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="4">
         <v>99</v>
       </c>
       <c r="E72" t="s">
@@ -25170,7 +25170,7 @@
         <v>1.01</v>
       </c>
       <c r="I72" s="1">
-        <f t="shared" ref="I72:I119" si="51">BJ72+(BK72-BJ72)*0.3</f>
+        <f t="shared" ref="I72" si="51">BJ72+(BK72-BJ72)*0.3</f>
         <v>5.5</v>
       </c>
       <c r="J72">
@@ -25478,16 +25478,16 @@
       </c>
     </row>
     <row r="73" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="4">
         <v>99</v>
       </c>
       <c r="E73" t="s">
@@ -25811,16 +25811,16 @@
       </c>
     </row>
     <row r="74" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D74" s="4">
         <v>96</v>
       </c>
       <c r="E74" t="s">
@@ -26144,16 +26144,16 @@
       </c>
     </row>
     <row r="75" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D75" s="4">
         <v>96</v>
       </c>
       <c r="E75" t="s">
@@ -26477,16 +26477,16 @@
       </c>
     </row>
     <row r="76" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D76" s="4">
         <v>101</v>
       </c>
       <c r="E76" t="s">
@@ -26810,16 +26810,16 @@
       </c>
     </row>
     <row r="77" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D77" s="4">
         <v>101</v>
       </c>
       <c r="E77" t="s">
@@ -27143,16 +27143,16 @@
       </c>
     </row>
     <row r="78" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D78" s="3">
+      <c r="D78" s="4">
         <v>98</v>
       </c>
       <c r="E78" t="s">
@@ -27476,16 +27476,16 @@
       </c>
     </row>
     <row r="79" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D79" s="4">
         <v>98</v>
       </c>
       <c r="E79" t="s">
@@ -27809,16 +27809,16 @@
       </c>
     </row>
     <row r="80" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D80" s="4">
         <v>100</v>
       </c>
       <c r="E80" t="s">
@@ -28142,16 +28142,16 @@
       </c>
     </row>
     <row r="81" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D81" s="4">
         <v>100</v>
       </c>
       <c r="E81" t="s">
@@ -28475,16 +28475,16 @@
       </c>
     </row>
     <row r="82" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D82" s="4">
         <v>96</v>
       </c>
       <c r="E82" t="s">
@@ -28808,16 +28808,16 @@
       </c>
     </row>
     <row r="83" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D83" s="4">
         <v>96</v>
       </c>
       <c r="E83" t="s">
@@ -29141,16 +29141,16 @@
       </c>
     </row>
     <row r="84" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D84" s="4">
         <v>105</v>
       </c>
       <c r="E84" t="s">
@@ -29474,16 +29474,16 @@
       </c>
     </row>
     <row r="85" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D85" s="4">
         <v>105</v>
       </c>
       <c r="E85" t="s">
@@ -29807,16 +29807,16 @@
       </c>
     </row>
     <row r="86" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C86" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D86" s="3">
+      <c r="D86" s="4">
         <v>102</v>
       </c>
       <c r="E86" t="s">
@@ -30140,16 +30140,16 @@
       </c>
     </row>
     <row r="87" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D87" s="3">
+      <c r="D87" s="4">
         <v>102</v>
       </c>
       <c r="E87" t="s">
@@ -30473,16 +30473,16 @@
       </c>
     </row>
     <row r="88" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D88" s="3">
+      <c r="D88" s="4">
         <v>103</v>
       </c>
       <c r="E88" t="s">
@@ -30806,16 +30806,16 @@
       </c>
     </row>
     <row r="89" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D89" s="3">
+      <c r="D89" s="4">
         <v>103</v>
       </c>
       <c r="E89" t="s">
@@ -31139,16 +31139,16 @@
       </c>
     </row>
     <row r="90" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C90" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D90" s="4">
         <v>100</v>
       </c>
       <c r="E90" t="s">
@@ -31472,16 +31472,16 @@
       </c>
     </row>
     <row r="91" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D91" s="4">
         <v>100</v>
       </c>
       <c r="E91" t="s">
@@ -31805,16 +31805,16 @@
       </c>
     </row>
     <row r="92" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C92" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D92" s="3">
+      <c r="D92" s="4">
         <v>99</v>
       </c>
       <c r="E92" t="s">
@@ -32138,16 +32138,16 @@
       </c>
     </row>
     <row r="93" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D93" s="3">
+      <c r="D93" s="4">
         <v>99</v>
       </c>
       <c r="E93" t="s">
@@ -32471,16 +32471,16 @@
       </c>
     </row>
     <row r="94" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D94" s="3">
+      <c r="D94" s="4">
         <v>104</v>
       </c>
       <c r="E94" t="s">
@@ -32804,16 +32804,16 @@
       </c>
     </row>
     <row r="95" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D95" s="3">
+      <c r="D95" s="4">
         <v>104</v>
       </c>
       <c r="E95" t="s">
@@ -32829,7 +32829,7 @@
         <v>0.44</v>
       </c>
       <c r="I95" s="1">
-        <f t="shared" ref="I95:I119" si="52">BJ95+(BK95-BJ95)*0.3</f>
+        <f t="shared" ref="I95" si="52">BJ95+(BK95-BJ95)*0.3</f>
         <v>4.0999999999999996</v>
       </c>
       <c r="J95">
@@ -33137,16 +33137,16 @@
       </c>
     </row>
     <row r="96" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D96" s="4">
         <v>96</v>
       </c>
       <c r="E96" t="s">
@@ -33470,16 +33470,16 @@
       </c>
     </row>
     <row r="97" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D97" s="4">
         <v>96</v>
       </c>
       <c r="E97" t="s">
@@ -33495,7 +33495,7 @@
         <v>1.58</v>
       </c>
       <c r="I97" s="1">
-        <f t="shared" ref="I97:I119" si="54">BJ97+(BK97-BJ97)*0.3</f>
+        <f t="shared" ref="I97" si="54">BJ97+(BK97-BJ97)*0.3</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="J97">
@@ -33803,16 +33803,16 @@
       </c>
     </row>
     <row r="98" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C98" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D98" s="3">
+      <c r="D98" s="4">
         <v>99</v>
       </c>
       <c r="E98" t="s">
@@ -33828,7 +33828,7 @@
         <v>1.49</v>
       </c>
       <c r="I98" s="1">
-        <f t="shared" ref="I98:I119" si="55">BJ98+(BL98-BJ98)*0.3</f>
+        <f t="shared" ref="I98" si="55">BJ98+(BL98-BJ98)*0.3</f>
         <v>2.5</v>
       </c>
       <c r="J98">
@@ -34136,16 +34136,16 @@
       </c>
     </row>
     <row r="99" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C99" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D99" s="4">
         <v>99</v>
       </c>
       <c r="E99" t="s">
@@ -34161,7 +34161,7 @@
         <v>1.65</v>
       </c>
       <c r="I99" s="1">
-        <f t="shared" ref="I99:I119" si="56">BJ99+(BK99-BJ99)*0.3</f>
+        <f t="shared" ref="I99" si="56">BJ99+(BK99-BJ99)*0.3</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="J99">
@@ -34469,16 +34469,16 @@
       </c>
     </row>
     <row r="100" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C100" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D100" s="4">
         <v>95</v>
       </c>
       <c r="E100" t="s">
@@ -34494,7 +34494,7 @@
         <v>1.73</v>
       </c>
       <c r="I100" s="1">
-        <f t="shared" ref="I100:I119" si="57">BJ100+(BL100-BJ100)*0.3</f>
+        <f t="shared" ref="I100" si="57">BJ100+(BL100-BJ100)*0.3</f>
         <v>1.2</v>
       </c>
       <c r="J100">
@@ -34802,16 +34802,16 @@
       </c>
     </row>
     <row r="101" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C101" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D101" s="3">
+      <c r="D101" s="4">
         <v>95</v>
       </c>
       <c r="E101" t="s">
@@ -34827,7 +34827,7 @@
         <v>1.8</v>
       </c>
       <c r="I101" s="1">
-        <f t="shared" ref="I101:I119" si="58">BJ101+(BK101-BJ101)*0.3</f>
+        <f t="shared" ref="I101" si="58">BJ101+(BK101-BJ101)*0.3</f>
         <v>5.6999999999999993</v>
       </c>
       <c r="J101">
@@ -35135,16 +35135,16 @@
       </c>
     </row>
     <row r="102" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C102" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D102" s="3">
+      <c r="D102" s="4">
         <v>94</v>
       </c>
       <c r="E102" t="s">
@@ -35160,7 +35160,7 @@
         <v>1.61</v>
       </c>
       <c r="I102" s="1">
-        <f t="shared" ref="I102:I119" si="59">BJ102+(BL102-BJ102)*0.3</f>
+        <f t="shared" ref="I102" si="59">BJ102+(BL102-BJ102)*0.3</f>
         <v>0.89999999999999991</v>
       </c>
       <c r="J102">
@@ -35468,16 +35468,16 @@
       </c>
     </row>
     <row r="103" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C103" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D103" s="3">
+      <c r="D103" s="4">
         <v>94</v>
       </c>
       <c r="E103" t="s">
@@ -35493,7 +35493,7 @@
         <v>0.74</v>
       </c>
       <c r="I103" s="1">
-        <f t="shared" ref="I103:I119" si="60">BJ103+(BK103-BJ103)*0.3</f>
+        <f t="shared" ref="I103" si="60">BJ103+(BK103-BJ103)*0.3</f>
         <v>5.6</v>
       </c>
       <c r="J103">
@@ -35801,16 +35801,16 @@
       </c>
     </row>
     <row r="104" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B104" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C104" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D104" s="3">
+      <c r="D104" s="4">
         <v>97</v>
       </c>
       <c r="E104" t="s">
@@ -35826,7 +35826,7 @@
         <v>1.88</v>
       </c>
       <c r="I104" s="1">
-        <f t="shared" ref="I104:I119" si="61">BJ104+(BL104-BJ104)*0.3</f>
+        <f t="shared" ref="I104" si="61">BJ104+(BL104-BJ104)*0.3</f>
         <v>0.6</v>
       </c>
       <c r="J104">
@@ -36134,16 +36134,16 @@
       </c>
     </row>
     <row r="105" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C105" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D105" s="3">
+      <c r="D105" s="4">
         <v>97</v>
       </c>
       <c r="E105" t="s">
@@ -36159,7 +36159,7 @@
         <v>0.91</v>
       </c>
       <c r="I105" s="1">
-        <f t="shared" ref="I105:I119" si="62">BJ105+(BK105-BJ105)*0.3</f>
+        <f t="shared" ref="I105" si="62">BJ105+(BK105-BJ105)*0.3</f>
         <v>5.6</v>
       </c>
       <c r="J105">
@@ -36467,16 +36467,16 @@
       </c>
     </row>
     <row r="106" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C106" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D106" s="3">
+      <c r="D106" s="4">
         <v>101</v>
       </c>
       <c r="E106" t="s">
@@ -36492,7 +36492,7 @@
         <v>2.89</v>
       </c>
       <c r="I106" s="1">
-        <f t="shared" ref="I106:I119" si="63">BJ106+(BL106-BJ106)*0.3</f>
+        <f t="shared" ref="I106" si="63">BJ106+(BL106-BJ106)*0.3</f>
         <v>4.9000000000000004</v>
       </c>
       <c r="J106">
@@ -36800,16 +36800,16 @@
       </c>
     </row>
     <row r="107" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B107" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C107" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D107" s="3">
+      <c r="D107" s="4">
         <v>101</v>
       </c>
       <c r="E107" t="s">
@@ -36825,7 +36825,7 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="I107" s="1">
-        <f t="shared" ref="I107:I119" si="64">BJ107+(BK107-BJ107)*0.3</f>
+        <f t="shared" ref="I107" si="64">BJ107+(BK107-BJ107)*0.3</f>
         <v>6.5</v>
       </c>
       <c r="J107">
@@ -37133,16 +37133,16 @@
       </c>
     </row>
     <row r="108" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C108" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D108" s="3">
+      <c r="D108" s="4">
         <v>104</v>
       </c>
       <c r="E108" t="s">
@@ -37158,7 +37158,7 @@
         <v>3.19</v>
       </c>
       <c r="I108" s="1">
-        <f t="shared" ref="I108:I119" si="65">BJ108+(BL108-BJ108)*0.3</f>
+        <f t="shared" ref="I108" si="65">BJ108+(BL108-BJ108)*0.3</f>
         <v>2.2999999999999998</v>
       </c>
       <c r="J108">
@@ -37466,16 +37466,16 @@
       </c>
     </row>
     <row r="109" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C109" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D109" s="3">
+      <c r="D109" s="4">
         <v>104</v>
       </c>
       <c r="E109" t="s">
@@ -37491,7 +37491,7 @@
         <v>1.46</v>
       </c>
       <c r="I109" s="1">
-        <f t="shared" ref="I109:I119" si="66">BJ109+(BK109-BJ109)*0.3</f>
+        <f t="shared" ref="I109" si="66">BJ109+(BK109-BJ109)*0.3</f>
         <v>10.6</v>
       </c>
       <c r="J109">
@@ -37799,16 +37799,16 @@
       </c>
     </row>
     <row r="110" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C110" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D110" s="3">
+      <c r="D110" s="4">
         <v>102</v>
       </c>
       <c r="E110" t="s">
@@ -37824,7 +37824,7 @@
         <v>1.53</v>
       </c>
       <c r="I110" s="1">
-        <f t="shared" ref="I110:I119" si="67">BJ110+(BL110-BJ110)*0.3</f>
+        <f t="shared" ref="I110" si="67">BJ110+(BL110-BJ110)*0.3</f>
         <v>4.8</v>
       </c>
       <c r="J110">
@@ -38132,16 +38132,16 @@
       </c>
     </row>
     <row r="111" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C111" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D111" s="3">
+      <c r="D111" s="4">
         <v>102</v>
       </c>
       <c r="E111" t="s">
@@ -38157,7 +38157,7 @@
         <v>2.65</v>
       </c>
       <c r="I111" s="1">
-        <f t="shared" ref="I111:I119" si="68">BJ111+(BK111-BJ111)*0.3</f>
+        <f t="shared" ref="I111" si="68">BJ111+(BK111-BJ111)*0.3</f>
         <v>5.3</v>
       </c>
       <c r="J111">
@@ -38465,16 +38465,16 @@
       </c>
     </row>
     <row r="112" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D112" s="3">
+      <c r="D112" s="4">
         <v>102</v>
       </c>
       <c r="E112" t="s">
@@ -38490,7 +38490,7 @@
         <v>1.26</v>
       </c>
       <c r="I112" s="1">
-        <f t="shared" ref="I112:I119" si="69">BJ112+(BL112-BJ112)*0.3</f>
+        <f t="shared" ref="I112" si="69">BJ112+(BL112-BJ112)*0.3</f>
         <v>5.5</v>
       </c>
       <c r="J112">
@@ -38798,16 +38798,16 @@
       </c>
     </row>
     <row r="113" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C113" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D113" s="4">
         <v>102</v>
       </c>
       <c r="E113" t="s">
@@ -38823,7 +38823,7 @@
         <v>2.86</v>
       </c>
       <c r="I113" s="1">
-        <f t="shared" ref="I113:I119" si="70">BJ113+(BK113-BJ113)*0.3</f>
+        <f t="shared" ref="I113" si="70">BJ113+(BK113-BJ113)*0.3</f>
         <v>2.8</v>
       </c>
       <c r="J113">
@@ -39131,16 +39131,16 @@
       </c>
     </row>
     <row r="114" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C114" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D114" s="4">
         <v>96</v>
       </c>
       <c r="E114" t="s">
@@ -39156,7 +39156,7 @@
         <v>1.08</v>
       </c>
       <c r="I114" s="1">
-        <f t="shared" ref="I114:I119" si="71">BJ114+(BL114-BJ114)*0.3</f>
+        <f t="shared" ref="I114" si="71">BJ114+(BL114-BJ114)*0.3</f>
         <v>0.89999999999999991</v>
       </c>
       <c r="J114">
@@ -39464,16 +39464,16 @@
       </c>
     </row>
     <row r="115" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C115" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D115" s="4">
         <v>96</v>
       </c>
       <c r="E115" t="s">
@@ -39489,7 +39489,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="I115" s="1">
-        <f t="shared" ref="I115:I119" si="72">BJ115+(BK115-BJ115)*0.3</f>
+        <f t="shared" ref="I115" si="72">BJ115+(BK115-BJ115)*0.3</f>
         <v>4.3</v>
       </c>
       <c r="J115">
@@ -39797,16 +39797,16 @@
       </c>
     </row>
     <row r="116" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
+      <c r="A116" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C116" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D116" s="4">
         <v>97</v>
       </c>
       <c r="E116" t="s">
@@ -39822,7 +39822,7 @@
         <v>1.73</v>
       </c>
       <c r="I116" s="1">
-        <f t="shared" ref="I116:I119" si="73">BJ116+(BL116-BJ116)*0.3</f>
+        <f t="shared" ref="I116:I117" si="73">BJ116+(BL116-BJ116)*0.3</f>
         <v>3.2</v>
       </c>
       <c r="J116">
@@ -40130,16 +40130,16 @@
       </c>
     </row>
     <row r="117" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C117" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D117" s="3">
+      <c r="D117" s="4">
         <v>97</v>
       </c>
       <c r="E117" t="s">
@@ -40463,16 +40463,16 @@
       </c>
     </row>
     <row r="118" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C118" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D118" s="3">
+      <c r="D118" s="4">
         <v>100</v>
       </c>
       <c r="E118" t="s">
@@ -40488,7 +40488,7 @@
         <v>1.45</v>
       </c>
       <c r="I118" s="1">
-        <f t="shared" ref="I118:I119" si="74">BJ118+(BK118-BJ118)*0.3</f>
+        <f t="shared" ref="I118" si="74">BJ118+(BK118-BJ118)*0.3</f>
         <v>2.1</v>
       </c>
       <c r="J118">
@@ -40796,16 +40796,16 @@
       </c>
     </row>
     <row r="119" spans="1:110" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C119" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D119" s="3">
+      <c r="D119" s="4">
         <v>100</v>
       </c>
       <c r="E119" t="s">
@@ -41130,249 +41130,6 @@
     </row>
   </sheetData>
   <mergeCells count="259">
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="AB1:AD1"/>
-    <mergeCell ref="AE1:AG1"/>
-    <mergeCell ref="AH1:AJ1"/>
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="AN1:AP1"/>
-    <mergeCell ref="AQ1:AS1"/>
-    <mergeCell ref="AT1:AV1"/>
-    <mergeCell ref="AW1:AY1"/>
-    <mergeCell ref="BB1:BD1"/>
-    <mergeCell ref="BF1:BH1"/>
-    <mergeCell ref="BK1:BM1"/>
-    <mergeCell ref="BN1:BP1"/>
-    <mergeCell ref="BQ1:BS1"/>
-    <mergeCell ref="BT1:BV1"/>
-    <mergeCell ref="CB1:CD1"/>
-    <mergeCell ref="CE1:CG1"/>
-    <mergeCell ref="CH1:CJ1"/>
-    <mergeCell ref="CK1:CM1"/>
-    <mergeCell ref="CN1:CP1"/>
-    <mergeCell ref="CQ1:CS1"/>
-    <mergeCell ref="CT1:CV1"/>
-    <mergeCell ref="CW1:CY1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="D102:D103"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="B110:B111"/>
-    <mergeCell ref="C110:C111"/>
-    <mergeCell ref="D110:D111"/>
     <mergeCell ref="A118:A119"/>
     <mergeCell ref="B118:B119"/>
     <mergeCell ref="C118:C119"/>
@@ -41389,6 +41146,249 @@
     <mergeCell ref="B116:B117"/>
     <mergeCell ref="C116:C117"/>
     <mergeCell ref="D116:D117"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="B106:B107"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="D110:D111"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="D102:D103"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="BT1:BV1"/>
+    <mergeCell ref="CB1:CD1"/>
+    <mergeCell ref="CE1:CG1"/>
+    <mergeCell ref="CH1:CJ1"/>
+    <mergeCell ref="CK1:CM1"/>
+    <mergeCell ref="CN1:CP1"/>
+    <mergeCell ref="CQ1:CS1"/>
+    <mergeCell ref="CT1:CV1"/>
+    <mergeCell ref="CW1:CY1"/>
+    <mergeCell ref="AN1:AP1"/>
+    <mergeCell ref="AQ1:AS1"/>
+    <mergeCell ref="AT1:AV1"/>
+    <mergeCell ref="AW1:AY1"/>
+    <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="BF1:BH1"/>
+    <mergeCell ref="BK1:BM1"/>
+    <mergeCell ref="BN1:BP1"/>
+    <mergeCell ref="BQ1:BS1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB1:AD1"/>
+    <mergeCell ref="AE1:AG1"/>
+    <mergeCell ref="AH1:AJ1"/>
+    <mergeCell ref="AK1:AM1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>